<commit_message>
B2C hotel booking flow and modification on cofig file for all env
</commit_message>
<xml_diff>
--- a/src/test/resources/Data.xlsx
+++ b/src/test/resources/Data.xlsx
@@ -7,6 +7,7 @@
     <sheet state="visible" name="DataForInternationHotel" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="DataWithHotelName" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="FlightEmployeeData" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="B2CHotelBookingData" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="51">
   <si>
     <t>City</t>
   </si>
@@ -100,6 +101,27 @@
     <t>DepatureDate</t>
   </si>
   <si>
+    <t>Flight Name</t>
+  </si>
+  <si>
+    <t>Price Type</t>
+  </si>
+  <si>
+    <t>AddOns</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>usernumber</t>
+  </si>
+  <si>
+    <t>userdate</t>
+  </si>
+  <si>
+    <t>usermob</t>
+  </si>
+  <si>
     <t>Vikas Yadav</t>
   </si>
   <si>
@@ -107,6 +129,45 @@
   </si>
   <si>
     <t>1</t>
+  </si>
+  <si>
+    <t>SpiceJet</t>
+  </si>
+  <si>
+    <t>Regular</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Vikas1234</t>
+  </si>
+  <si>
+    <t>vikas1234</t>
+  </si>
+  <si>
+    <t>Jan 2024 20</t>
+  </si>
+  <si>
+    <t>CheckInDate</t>
+  </si>
+  <si>
+    <t>CheckOutdate</t>
+  </si>
+  <si>
+    <t>Guest</t>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
+    <t>Jan 2024 22</t>
+  </si>
+  <si>
+    <t>Jan 2024 25</t>
+  </si>
+  <si>
+    <t>1 Guest</t>
   </si>
 </sst>
 </file>
@@ -156,7 +217,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -175,6 +236,9 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -196,6 +260,10 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -656,7 +724,7 @@
     <col customWidth="1" min="3" max="3" width="18.88"/>
     <col customWidth="1" min="5" max="5" width="20.75"/>
     <col customWidth="1" min="6" max="6" width="18.88"/>
-    <col customWidth="1" min="7" max="7" width="27.0"/>
+    <col customWidth="1" min="7" max="8" width="27.0"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -681,6 +749,30 @@
       <c r="G1" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
@@ -690,19 +782,91 @@
         <v>16</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>13</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="19.63"/>
+    <col customWidth="1" min="2" max="2" width="17.0"/>
+    <col customWidth="1" min="3" max="3" width="15.75"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>